<commit_message>
Updated hyperlinks for the more recent reviews.
</commit_message>
<xml_diff>
--- a/Wireless Earbuds Reviews.xlsx
+++ b/Wireless Earbuds Reviews.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ceba4c9e644e6e6/YouTube/Share/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ceba4c9e644e6e6/YouTube/Earbuds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2637" documentId="8_{32C462A0-5FFE-4E26-81A4-9140FB4F6073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4104197A-B239-4661-B52D-5921650BCA44}"/>
+  <xr:revisionPtr revIDLastSave="2653" documentId="8_{32C462A0-5FFE-4E26-81A4-9140FB4F6073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB0BE81C-ABE6-47AD-8A6C-213C78234722}"/>
   <bookViews>
-    <workbookView xWindow="14865" yWindow="7845" windowWidth="31035" windowHeight="23985" xr2:uid="{635816C2-857D-4EAE-95AA-796751DEB26C}"/>
+    <workbookView xWindow="16350" yWindow="6420" windowWidth="31035" windowHeight="23985" xr2:uid="{635816C2-857D-4EAE-95AA-796751DEB26C}"/>
   </bookViews>
   <sheets>
     <sheet name="Ranking" sheetId="21" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <sheet name="EarFun Air Pro 4" sheetId="36" r:id="rId15"/>
     <sheet name="Nothing CMF Buds Pro 2" sheetId="37" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,39 +53,288 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="114">
   <si>
+    <t>Ranking</t>
+  </si>
+  <si>
+    <t>Earbud</t>
+  </si>
+  <si>
+    <t>Sound Score</t>
+  </si>
+  <si>
+    <t>Mic Score</t>
+  </si>
+  <si>
+    <t>My Cost</t>
+  </si>
+  <si>
+    <t>My Sound QC</t>
+  </si>
+  <si>
+    <t>My Mic QC</t>
+  </si>
+  <si>
+    <t>Usual Cost</t>
+  </si>
+  <si>
+    <t>Usual Sound QC</t>
+  </si>
+  <si>
+    <t>Usual Mic QC</t>
+  </si>
+  <si>
+    <t>Mic Review</t>
+  </si>
+  <si>
+    <t>Review Link (EN)</t>
+  </si>
+  <si>
+    <t>Review Link (PT)</t>
+  </si>
+  <si>
+    <t>SoundPeats Engine 4</t>
+  </si>
+  <si>
+    <t>https://youtu.be/JmYYoLVEvD4</t>
+  </si>
+  <si>
+    <t>https://youtu.be/PWNI0eVP3N0</t>
+  </si>
+  <si>
+    <t>https://youtu.be/UZQKtcEeGg8</t>
+  </si>
+  <si>
+    <t>Soundcore Liberty 3 Pro</t>
+  </si>
+  <si>
+    <t>https://youtu.be/wSBMf8o41o4</t>
+  </si>
+  <si>
+    <t>https://youtu.be/BG9Fz0IOJT0</t>
+  </si>
+  <si>
+    <t>https://youtu.be/11mN3KduHiE</t>
+  </si>
+  <si>
+    <t>realme Buds Air 5 Pro</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Gg2aZm3YZNo</t>
+  </si>
+  <si>
+    <t>https://youtu.be/9a4Lynl_AEk</t>
+  </si>
+  <si>
+    <t>https://youtu.be/9vrwHu7uHZM</t>
+  </si>
+  <si>
+    <t>Nothing CMF Buds Pro 2</t>
+  </si>
+  <si>
+    <t>https://youtu.be/L3xvcN5Qk80</t>
+  </si>
+  <si>
+    <t>https://youtu.be/u5Huf04KjmA</t>
+  </si>
+  <si>
+    <t>https://youtu.be/P9Co986Ugfw</t>
+  </si>
+  <si>
+    <t>Technics AZ60</t>
+  </si>
+  <si>
+    <t>https://youtu.be/cRcq3tdonVY</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Z8-xXW5Rq_I</t>
+  </si>
+  <si>
+    <t>https://youtu.be/dwP26d7eTQU</t>
+  </si>
+  <si>
+    <t>EarFun Air Pro 4</t>
+  </si>
+  <si>
+    <t>https://youtu.be/91kLw-7N3rE</t>
+  </si>
+  <si>
+    <t>https://youtu.be/d9wF2JgkzNw</t>
+  </si>
+  <si>
+    <t>https://youtu.be/CG0eXc_AjmY</t>
+  </si>
+  <si>
+    <t>Soundcore Liberty 4 NC</t>
+  </si>
+  <si>
+    <t>https://youtu.be/K0cfS3sUFsM</t>
+  </si>
+  <si>
+    <t>https://youtu.be/5lCNIzErOSU</t>
+  </si>
+  <si>
+    <t>https://youtu.be/3hvHo_kF9mw</t>
+  </si>
+  <si>
+    <t>SoundPeats Air4 Pro</t>
+  </si>
+  <si>
+    <t>https://youtu.be/cQ3dEKNXAkA</t>
+  </si>
+  <si>
+    <t>https://youtu.be/XqekBEyURUs</t>
+  </si>
+  <si>
+    <t>https://youtu.be/wQtQIgk5E9g</t>
+  </si>
+  <si>
+    <t>1MORE PistonBuds Pro Q30</t>
+  </si>
+  <si>
+    <t>https://youtu.be/8C2YWBoW5TY</t>
+  </si>
+  <si>
+    <t>https://youtu.be/nE0m088qjJA</t>
+  </si>
+  <si>
+    <t>https://youtu.be/I_CzD8Rm5cU</t>
+  </si>
+  <si>
+    <t>Edifier W240TN</t>
+  </si>
+  <si>
+    <t>https://youtu.be/BzV6WPd1Bds</t>
+  </si>
+  <si>
+    <t>https://youtu.be/NvhhcoLgVFs</t>
+  </si>
+  <si>
+    <t>https://youtu.be/egX8-Eue4WY</t>
+  </si>
+  <si>
+    <t>Baseus Bowie MA10</t>
+  </si>
+  <si>
+    <t>https://youtu.be/UaIPcv9J09U</t>
+  </si>
+  <si>
+    <t>https://youtu.be/mvDwWCCuHsM</t>
+  </si>
+  <si>
+    <t>https://youtu.be/QEvYTHcL2TM</t>
+  </si>
+  <si>
+    <t>Tozo NC9 2024</t>
+  </si>
+  <si>
+    <t>https://youtu.be/b4yzSfAEnUM</t>
+  </si>
+  <si>
+    <t>https://youtu.be/WWIDbFzHSaQ</t>
+  </si>
+  <si>
+    <t>https://youtu.be/gUXGBsT4nHM</t>
+  </si>
+  <si>
+    <t>Tozo Crystal Pods</t>
+  </si>
+  <si>
+    <t>https://youtu.be/RyEucysc0xQ</t>
+  </si>
+  <si>
+    <t>https://youtu.be/hhg9MeVyvV8</t>
+  </si>
+  <si>
+    <t>https://youtu.be/BvQf3131M-c</t>
+  </si>
+  <si>
+    <t>Soundcore Liberty 4</t>
+  </si>
+  <si>
+    <t>https://youtu.be/hrjaL77REA4</t>
+  </si>
+  <si>
+    <t>https://youtu.be/xOAW-A6YjnU</t>
+  </si>
+  <si>
+    <t>https://youtu.be/SI1qichCE3M</t>
+  </si>
+  <si>
+    <t>Jabra Elite 4 Active</t>
+  </si>
+  <si>
+    <t>https://youtu.be/BmebJI9H5tk</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Zu5FmrEzIs0</t>
+  </si>
+  <si>
+    <t>https://youtu.be/pgKKPVRwt0Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Aspect</t>
+  </si>
+  <si>
     <t>Weight</t>
   </si>
   <si>
+    <t>Score (0-10)</t>
+  </si>
+  <si>
+    <t>Weighted Score</t>
+  </si>
+  <si>
+    <t>Listening Score</t>
+  </si>
+  <si>
+    <t>Critical (75%)</t>
+  </si>
+  <si>
+    <t>Sound quality</t>
+  </si>
+  <si>
+    <t>Comfort (buds + case)</t>
+  </si>
+  <si>
     <t>Volume</t>
   </si>
   <si>
+    <t>Other (25%)</t>
+  </si>
+  <si>
     <t>Battery life</t>
   </si>
   <si>
     <t>ANC</t>
   </si>
   <si>
+    <t>Eartip replacement</t>
+  </si>
+  <si>
     <t>Custom EQ</t>
   </si>
   <si>
-    <t>Eartip replacement</t>
+    <t>Control usability / range</t>
+  </si>
+  <si>
+    <t>Hi-Res codecs</t>
+  </si>
+  <si>
+    <t>Multi-Point</t>
+  </si>
+  <si>
+    <t>Gaming mode</t>
   </si>
   <si>
     <t>Control customization</t>
   </si>
   <si>
-    <t>Hi-Res codecs</t>
-  </si>
-  <si>
     <t>Fast charging</t>
   </si>
   <si>
-    <t>Gaming mode</t>
-  </si>
-  <si>
-    <t>Multi-Point</t>
-  </si>
-  <si>
     <t>Find my device</t>
   </si>
   <si>
@@ -95,304 +344,55 @@
     <t>Wireless charging</t>
   </si>
   <si>
-    <t>Score (0-10)</t>
-  </si>
-  <si>
-    <t>Comfort (buds + case)</t>
-  </si>
-  <si>
-    <t>Control usability / range</t>
+    <t>Microphone Score</t>
   </si>
   <si>
     <t>Microphone / Call quality</t>
   </si>
   <si>
-    <t>Microphone Score</t>
-  </si>
-  <si>
-    <t>Sound quality</t>
-  </si>
-  <si>
-    <t>Listening Score</t>
-  </si>
-  <si>
-    <t>Aspect</t>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Mono Mode</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
   <si>
     <t>Listening</t>
   </si>
   <si>
-    <t>Critical (75%)</t>
-  </si>
-  <si>
-    <t>Other (25%)</t>
-  </si>
-  <si>
     <t>Microphone</t>
   </si>
   <si>
-    <t>Weighted Score</t>
+    <t>IP Rating</t>
+  </si>
+  <si>
+    <t>IPX4</t>
   </si>
   <si>
     <t>Cost per Quality</t>
   </si>
   <si>
-    <t>My Cost</t>
-  </si>
-  <si>
-    <t>Usual Cost</t>
-  </si>
-  <si>
-    <t>Mic Score</t>
-  </si>
-  <si>
-    <t>Sound Score</t>
-  </si>
-  <si>
-    <t>Earbud</t>
-  </si>
-  <si>
-    <t>SoundPeats Engine 4</t>
-  </si>
-  <si>
-    <t>Edifier W240TN</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Usual Sound QC</t>
-  </si>
-  <si>
-    <t>Usual Mic QC</t>
-  </si>
-  <si>
-    <t>My Sound QC</t>
-  </si>
-  <si>
-    <t>My Mic QC</t>
-  </si>
-  <si>
-    <t>Mono Mode</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>1MORE PistonBuds Pro Q30</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>IP Rating</t>
-  </si>
-  <si>
-    <t>IPX4</t>
-  </si>
-  <si>
     <t>IP55</t>
   </si>
   <si>
     <t>IPX5</t>
   </si>
   <si>
-    <t>https://youtu.be/nE0m088qjJA</t>
-  </si>
-  <si>
-    <t>Review Link (EN)</t>
-  </si>
-  <si>
-    <t>Review Link (PT)</t>
-  </si>
-  <si>
-    <t>https://youtu.be/I_CzD8Rm5cU</t>
-  </si>
-  <si>
-    <t>https://youtu.be/NvhhcoLgVFs</t>
-  </si>
-  <si>
-    <t>https://youtu.be/egX8-Eue4WY</t>
-  </si>
-  <si>
-    <t>https://youtu.be/UZQKtcEeGg8</t>
-  </si>
-  <si>
-    <t>https://youtu.be/PWNI0eVP3N0</t>
-  </si>
-  <si>
-    <t>Technics AZ60</t>
-  </si>
-  <si>
-    <t>https://youtu.be/dwP26d7eTQU</t>
-  </si>
-  <si>
-    <t>https://youtu.be/Z8-xXW5Rq_I</t>
-  </si>
-  <si>
-    <t>Mic Review</t>
-  </si>
-  <si>
-    <t>https://youtu.be/cRcq3tdonVY</t>
-  </si>
-  <si>
-    <t>https://youtu.be/8C2YWBoW5TY</t>
-  </si>
-  <si>
-    <t>https://youtu.be/JmYYoLVEvD4</t>
-  </si>
-  <si>
-    <t>https://youtu.be/BzV6WPd1Bds</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>Soundcore Liberty 3 Pro</t>
-  </si>
-  <si>
-    <t>https://youtu.be/wSBMf8o41o4</t>
-  </si>
-  <si>
-    <t>https://youtu.be/BG9Fz0IOJT0</t>
-  </si>
-  <si>
-    <t>https://youtu.be/11mN3KduHiE</t>
-  </si>
-  <si>
-    <t>Soundcore Liberty 4</t>
-  </si>
-  <si>
-    <t>https://youtu.be/hrjaL77REA4</t>
-  </si>
-  <si>
-    <t>https://youtu.be/xOAW-A6YjnU</t>
-  </si>
-  <si>
-    <t>https://youtu.be/SI1qichCE3M</t>
-  </si>
-  <si>
     <t>IP57</t>
   </si>
   <si>
-    <t>Jabra Elite 4 Active</t>
-  </si>
-  <si>
-    <t>https://youtu.be/BmebJI9H5tk</t>
-  </si>
-  <si>
-    <t>https://youtu.be/Zu5FmrEzIs0</t>
-  </si>
-  <si>
-    <t>https://youtu.be/pgKKPVRwt0Y</t>
-  </si>
-  <si>
-    <t>Soundcore Liberty 4 NC</t>
-  </si>
-  <si>
-    <t>https://youtu.be/K0cfS3sUFsM</t>
-  </si>
-  <si>
-    <t>https://youtu.be/5lCNIzErOSU</t>
-  </si>
-  <si>
-    <t>https://youtu.be/3hvHo_kF9mw</t>
-  </si>
-  <si>
     <t>IPX6</t>
   </si>
   <si>
-    <t>Baseus Bowie MA10</t>
-  </si>
-  <si>
-    <t>https://youtu.be/UaIPcv9J09U</t>
-  </si>
-  <si>
-    <t>https://youtu.be/QEvYTHcL2TM</t>
-  </si>
-  <si>
-    <t>https://youtu.be/mvDwWCCuHsM</t>
-  </si>
-  <si>
-    <t>SoundPeats Air4 Pro</t>
-  </si>
-  <si>
-    <t>https://youtu.be/cQ3dEKNXAkA</t>
-  </si>
-  <si>
-    <t>https://youtu.be/XqekBEyURUs</t>
-  </si>
-  <si>
-    <t>https://youtu.be/wQtQIgk5E9g</t>
-  </si>
-  <si>
-    <t>realme Buds Air 5 Pro</t>
-  </si>
-  <si>
-    <t>https://youtu.be/Gg2aZm3YZNo</t>
-  </si>
-  <si>
-    <t>https://youtu.be/9vrwHu7uHZM</t>
-  </si>
-  <si>
-    <t>https://youtu.be/9a4Lynl_AEk</t>
-  </si>
-  <si>
     <t>IPX8</t>
-  </si>
-  <si>
-    <t>Tozo NC9 2024</t>
-  </si>
-  <si>
-    <t>Tozo Crystal Pods</t>
-  </si>
-  <si>
-    <t>EarFun Air Pro 4</t>
-  </si>
-  <si>
-    <t>Nothing CMF Buds Pro 2</t>
-  </si>
-  <si>
-    <t>Ranking</t>
-  </si>
-  <si>
-    <t>https://youtu.be/b4yzSfAEnUM</t>
-  </si>
-  <si>
-    <t>https://youtu.be/RyEucysc0xQ</t>
-  </si>
-  <si>
-    <t>https://youtu.be/91kLw-7N3rE</t>
-  </si>
-  <si>
-    <t>https://youtu.be/L3xvcN5Qk80</t>
-  </si>
-  <si>
-    <t>https://youtu.be/WWIDbFzHSaQ</t>
-  </si>
-  <si>
-    <t>https://youtu.be/gUXGBsT4nHM</t>
-  </si>
-  <si>
-    <t>https://youtu.be/hhg9MeVyvV8</t>
-  </si>
-  <si>
-    <t>https://youtu.be/BvQf3131M-c</t>
-  </si>
-  <si>
-    <t>https://youtu.be/d9wF2JgkzNw</t>
-  </si>
-  <si>
-    <t>https://youtu.be/CG0eXc_AjmY</t>
-  </si>
-  <si>
-    <t>https://youtu.be/u5Huf04KjmA</t>
-  </si>
-  <si>
-    <t>https://youtu.be/P9Co986Ugfw</t>
   </si>
 </sst>
 </file>
@@ -1884,7 +1884,7 @@
   <dimension ref="A1:M68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,43 +1906,43 @@
   <sheetData>
     <row r="1" spans="1:13" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="H1" s="42" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="I1" s="42" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="J1" s="42" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="K1" s="43" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="L1" s="43" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="M1" s="45" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -1951,7 +1951,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C2" s="26">
         <f>'SoundPeats Engine 4'!$J$21</f>
@@ -1986,13 +1986,13 @@
         <v>10.4</v>
       </c>
       <c r="K2" s="47" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="L2" s="47" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="M2" s="48" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -2001,7 +2001,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="C3" s="26">
         <f>'Soundcore Liberty 3 Pro'!$J$21</f>
@@ -2036,13 +2036,13 @@
         <v>17.5</v>
       </c>
       <c r="K3" s="47" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="L3" s="47" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="M3" s="48" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -2051,7 +2051,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>92</v>
+        <v>21</v>
       </c>
       <c r="C4" s="26">
         <f>'realme Buds Air 5 Pro'!$J$21</f>
@@ -2086,13 +2086,13 @@
         <v>8.4210526315789469</v>
       </c>
       <c r="K4" s="47" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="L4" s="47" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
       <c r="M4" s="48" t="s">
-        <v>94</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -2101,7 +2101,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="C5" s="33">
         <f>'Nothing CMF Buds Pro 2'!$J$21</f>
@@ -2136,13 +2136,13 @@
         <v>6.875</v>
       </c>
       <c r="K5" s="50" t="s">
-        <v>105</v>
+        <v>26</v>
       </c>
       <c r="L5" s="50" t="s">
-        <v>112</v>
-      </c>
-      <c r="M5" s="51" t="s">
-        <v>113</v>
+        <v>27</v>
+      </c>
+      <c r="M5" s="50" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -2151,7 +2151,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="C6" s="33">
         <f>'Technics AZ60'!$J$21</f>
@@ -2186,13 +2186,13 @@
         <v>32.857142857142854</v>
       </c>
       <c r="K6" s="50" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="L6" s="50" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="M6" s="51" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -2201,7 +2201,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>99</v>
+        <v>33</v>
       </c>
       <c r="C7" s="33">
         <f>'EarFun Air Pro 4'!$J$21</f>
@@ -2236,13 +2236,13 @@
         <v>10</v>
       </c>
       <c r="K7" s="50" t="s">
-        <v>104</v>
+        <v>34</v>
       </c>
       <c r="L7" s="50" t="s">
-        <v>110</v>
-      </c>
-      <c r="M7" s="51" t="s">
-        <v>111</v>
+        <v>35</v>
+      </c>
+      <c r="M7" s="50" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -2251,7 +2251,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="C8" s="33">
         <f>'Soundcore Liberty 4 NC'!$J$21</f>
@@ -2286,13 +2286,13 @@
         <v>11.25</v>
       </c>
       <c r="K8" s="50" t="s">
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="L8" s="50" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="M8" s="51" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -2301,7 +2301,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="C9" s="33">
         <f>'SoundPeats Air4 Pro'!$J$21</f>
@@ -2336,13 +2336,13 @@
         <v>10</v>
       </c>
       <c r="K9" s="50" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="L9" s="50" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="M9" s="51" t="s">
-        <v>91</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -2351,7 +2351,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C10" s="33">
         <f>'1MORE PistonBuds Pro Q30'!$J$21</f>
@@ -2386,13 +2386,13 @@
         <v>6.875</v>
       </c>
       <c r="K10" s="50" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="L10" s="50" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M10" s="51" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -2401,7 +2401,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C11" s="33">
         <f>'Edifier W240TN'!$J$21</f>
@@ -2436,13 +2436,13 @@
         <v>13.333333333333334</v>
       </c>
       <c r="K11" s="50" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="L11" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M11" s="51" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -2451,7 +2451,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="C12" s="33">
         <f>'Baseus Bowie MA10'!$J$21</f>
@@ -2486,13 +2486,13 @@
         <v>4.2857142857142856</v>
       </c>
       <c r="K12" s="50" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="L12" s="50" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="M12" s="51" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -2501,7 +2501,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="C13" s="33">
         <f>'Tozo NC9 2024'!$J$21</f>
@@ -2536,13 +2536,13 @@
         <v>8</v>
       </c>
       <c r="K13" s="50" t="s">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="L13" s="50" t="s">
-        <v>106</v>
-      </c>
-      <c r="M13" s="51" t="s">
-        <v>107</v>
+        <v>59</v>
+      </c>
+      <c r="M13" s="50" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -2551,7 +2551,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="C14" s="33">
         <f>'Tozo Crystal Pods'!$J$21</f>
@@ -2586,13 +2586,13 @@
         <v>5</v>
       </c>
       <c r="K14" s="50" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="L14" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="M14" s="51" t="s">
-        <v>109</v>
+        <v>63</v>
+      </c>
+      <c r="M14" s="50" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -2601,7 +2601,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C15" s="33">
         <f>'Soundcore Liberty 4'!$J$21</f>
@@ -2636,13 +2636,13 @@
         <v>16.666666666666668</v>
       </c>
       <c r="K15" s="50" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="L15" s="50" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="M15" s="51" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -2651,7 +2651,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C16" s="33">
         <f>'Jabra Elite 4 Active'!$J$21</f>
@@ -2686,18 +2686,18 @@
         <v>17.142857142857142</v>
       </c>
       <c r="K16" s="50" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L16" s="50" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="M16" s="51" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="F17" s="12"/>
     </row>
@@ -2887,11 +2887,23 @@
     <hyperlink ref="K9" r:id="rId28" xr:uid="{E94E9EB5-14BA-4BE8-A214-E57D5F2CB686}"/>
     <hyperlink ref="L9" r:id="rId29" xr:uid="{56113573-F9AC-4991-8720-2FAAF9BEF633}"/>
     <hyperlink ref="M9" r:id="rId30" xr:uid="{0B200221-1390-419A-AD67-23E26424B0EC}"/>
+    <hyperlink ref="K5" r:id="rId31" xr:uid="{EB27987B-A44E-4D78-849E-AE70EBD575F1}"/>
+    <hyperlink ref="L5" r:id="rId32" xr:uid="{A4951CDA-AAEE-4612-9613-CD11C0923F37}"/>
+    <hyperlink ref="M5" r:id="rId33" xr:uid="{E5BCB2A1-3206-4A27-9A0B-D8AEFCDA6216}"/>
+    <hyperlink ref="K7" r:id="rId34" xr:uid="{5E97F280-9915-4EAB-8673-32636200A675}"/>
+    <hyperlink ref="L7" r:id="rId35" xr:uid="{06200978-5DD6-484E-ABD8-3AFF681FEED6}"/>
+    <hyperlink ref="M7" r:id="rId36" xr:uid="{12D48F5A-1E1E-4965-A521-43316420C776}"/>
+    <hyperlink ref="K13" r:id="rId37" xr:uid="{B871EC08-2D20-4FA5-B5A1-0604FDE09D52}"/>
+    <hyperlink ref="L13" r:id="rId38" xr:uid="{058A27E5-4610-4A6A-8C41-68AFB42ADB32}"/>
+    <hyperlink ref="M13" r:id="rId39" xr:uid="{FC1FACDC-52FE-46F0-9E98-DB86330DA9A3}"/>
+    <hyperlink ref="K14" r:id="rId40" xr:uid="{5FEE32C4-E43E-486B-8294-43FAB04BEBAC}"/>
+    <hyperlink ref="L14" r:id="rId41" xr:uid="{62C321BF-DD0B-4137-B8BA-3A3FC84191CC}"/>
+    <hyperlink ref="M14" r:id="rId42" xr:uid="{A4110B7D-3902-4E40-94EA-935756C4F4E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId31"/>
+  <pageSetup orientation="portrait" r:id="rId43"/>
   <tableParts count="1">
-    <tablePart r:id="rId32"/>
+    <tablePart r:id="rId44"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2921,27 +2933,27 @@
       <c r="A1" s="60"/>
       <c r="B1" s="61"/>
       <c r="C1" s="11" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="D2" s="8">
         <v>0.5</v>
@@ -2958,7 +2970,7 @@
       <c r="A3" s="63"/>
       <c r="B3" s="65"/>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D3" s="8">
         <v>0.15</v>
@@ -2975,7 +2987,7 @@
       <c r="A4" s="63"/>
       <c r="B4" s="65"/>
       <c r="C4" s="7" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D4" s="8">
         <v>0.1</v>
@@ -2991,10 +3003,10 @@
     <row r="5" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
       <c r="B5" s="66" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D5" s="10">
         <v>0.04</v>
@@ -3011,7 +3023,7 @@
       <c r="A6" s="63"/>
       <c r="B6" s="66"/>
       <c r="C6" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="D6" s="10">
         <v>0.03</v>
@@ -3028,7 +3040,7 @@
       <c r="A7" s="63"/>
       <c r="B7" s="66"/>
       <c r="C7" s="9" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D7" s="10">
         <v>0.03</v>
@@ -3045,7 +3057,7 @@
       <c r="A8" s="63"/>
       <c r="B8" s="66"/>
       <c r="C8" s="9" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="D8" s="10">
         <v>0.02</v>
@@ -3062,7 +3074,7 @@
       <c r="A9" s="63"/>
       <c r="B9" s="66"/>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="D9" s="10">
         <v>0.02</v>
@@ -3079,7 +3091,7 @@
       <c r="A10" s="63"/>
       <c r="B10" s="66"/>
       <c r="C10" s="9" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D10" s="10">
         <v>0.02</v>
@@ -3096,7 +3108,7 @@
       <c r="A11" s="63"/>
       <c r="B11" s="66"/>
       <c r="C11" s="9" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D11" s="10">
         <v>0.02</v>
@@ -3113,7 +3125,7 @@
       <c r="A12" s="63"/>
       <c r="B12" s="66"/>
       <c r="C12" s="9" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D12" s="10">
         <v>0.02</v>
@@ -3130,7 +3142,7 @@
       <c r="A13" s="63"/>
       <c r="B13" s="66"/>
       <c r="C13" s="9" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="D13" s="10">
         <v>0.01</v>
@@ -3147,7 +3159,7 @@
       <c r="A14" s="63"/>
       <c r="B14" s="66"/>
       <c r="C14" s="9" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="D14" s="10">
         <v>0.01</v>
@@ -3164,7 +3176,7 @@
       <c r="A15" s="63"/>
       <c r="B15" s="66"/>
       <c r="C15" s="9" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="D15" s="10">
         <v>0.01</v>
@@ -3181,7 +3193,7 @@
       <c r="A16" s="63"/>
       <c r="B16" s="66"/>
       <c r="C16" s="9" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="D16" s="10">
         <v>0.01</v>
@@ -3198,7 +3210,7 @@
       <c r="A17" s="64"/>
       <c r="B17" s="66"/>
       <c r="C17" s="9" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="D17" s="10">
         <v>0.01</v>
@@ -3213,11 +3225,11 @@
     </row>
     <row r="18" spans="1:11" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="67" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="B18" s="68"/>
       <c r="C18" s="6" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="D18" s="5">
         <v>1</v>
@@ -3240,34 +3252,34 @@
     </row>
     <row r="20" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="I20" s="57" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A21" s="69"/>
       <c r="B21" s="24" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -3291,10 +3303,10 @@
       <c r="F22" s="2"/>
       <c r="I22" s="59"/>
       <c r="J22" s="19" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
@@ -3363,7 +3375,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3383,27 +3395,27 @@
       <c r="A1" s="60"/>
       <c r="B1" s="61"/>
       <c r="C1" s="11" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="D2" s="8">
         <v>0.5</v>
@@ -3420,7 +3432,7 @@
       <c r="A3" s="63"/>
       <c r="B3" s="65"/>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D3" s="8">
         <v>0.15</v>
@@ -3437,7 +3449,7 @@
       <c r="A4" s="63"/>
       <c r="B4" s="65"/>
       <c r="C4" s="7" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D4" s="8">
         <v>0.1</v>
@@ -3453,10 +3465,10 @@
     <row r="5" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
       <c r="B5" s="66" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D5" s="10">
         <v>0.04</v>
@@ -3473,7 +3485,7 @@
       <c r="A6" s="63"/>
       <c r="B6" s="66"/>
       <c r="C6" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="D6" s="10">
         <v>0.03</v>
@@ -3490,7 +3502,7 @@
       <c r="A7" s="63"/>
       <c r="B7" s="66"/>
       <c r="C7" s="9" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D7" s="10">
         <v>0.03</v>
@@ -3507,7 +3519,7 @@
       <c r="A8" s="63"/>
       <c r="B8" s="66"/>
       <c r="C8" s="9" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="D8" s="10">
         <v>0.02</v>
@@ -3524,7 +3536,7 @@
       <c r="A9" s="63"/>
       <c r="B9" s="66"/>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="D9" s="10">
         <v>0.02</v>
@@ -3541,7 +3553,7 @@
       <c r="A10" s="63"/>
       <c r="B10" s="66"/>
       <c r="C10" s="9" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D10" s="10">
         <v>0.02</v>
@@ -3558,7 +3570,7 @@
       <c r="A11" s="63"/>
       <c r="B11" s="66"/>
       <c r="C11" s="9" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D11" s="10">
         <v>0.02</v>
@@ -3575,7 +3587,7 @@
       <c r="A12" s="63"/>
       <c r="B12" s="66"/>
       <c r="C12" s="9" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D12" s="10">
         <v>0.02</v>
@@ -3592,7 +3604,7 @@
       <c r="A13" s="63"/>
       <c r="B13" s="66"/>
       <c r="C13" s="9" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="D13" s="10">
         <v>0.01</v>
@@ -3609,7 +3621,7 @@
       <c r="A14" s="63"/>
       <c r="B14" s="66"/>
       <c r="C14" s="9" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="D14" s="10">
         <v>0.01</v>
@@ -3626,7 +3638,7 @@
       <c r="A15" s="63"/>
       <c r="B15" s="66"/>
       <c r="C15" s="9" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="D15" s="10">
         <v>0.01</v>
@@ -3643,7 +3655,7 @@
       <c r="A16" s="63"/>
       <c r="B16" s="66"/>
       <c r="C16" s="9" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="D16" s="10">
         <v>0.01</v>
@@ -3660,7 +3672,7 @@
       <c r="A17" s="64"/>
       <c r="B17" s="66"/>
       <c r="C17" s="9" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="D17" s="10">
         <v>0.01</v>
@@ -3675,11 +3687,11 @@
     </row>
     <row r="18" spans="1:11" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="67" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="B18" s="68"/>
       <c r="C18" s="6" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="D18" s="5">
         <v>1</v>
@@ -3702,34 +3714,34 @@
     </row>
     <row r="20" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="I20" s="57" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A21" s="69"/>
       <c r="B21" s="24" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -3753,10 +3765,10 @@
       <c r="F22" s="2"/>
       <c r="I22" s="59"/>
       <c r="J22" s="19" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
@@ -3845,27 +3857,27 @@
       <c r="A1" s="60"/>
       <c r="B1" s="61"/>
       <c r="C1" s="11" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="D2" s="8">
         <v>0.5</v>
@@ -3882,7 +3894,7 @@
       <c r="A3" s="63"/>
       <c r="B3" s="65"/>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D3" s="8">
         <v>0.15</v>
@@ -3899,7 +3911,7 @@
       <c r="A4" s="63"/>
       <c r="B4" s="65"/>
       <c r="C4" s="7" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D4" s="8">
         <v>0.1</v>
@@ -3915,10 +3927,10 @@
     <row r="5" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
       <c r="B5" s="66" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D5" s="10">
         <v>0.04</v>
@@ -3935,7 +3947,7 @@
       <c r="A6" s="63"/>
       <c r="B6" s="66"/>
       <c r="C6" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="D6" s="10">
         <v>0.03</v>
@@ -3952,7 +3964,7 @@
       <c r="A7" s="63"/>
       <c r="B7" s="66"/>
       <c r="C7" s="9" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D7" s="10">
         <v>0.03</v>
@@ -3969,7 +3981,7 @@
       <c r="A8" s="63"/>
       <c r="B8" s="66"/>
       <c r="C8" s="9" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="D8" s="10">
         <v>0.02</v>
@@ -3986,7 +3998,7 @@
       <c r="A9" s="63"/>
       <c r="B9" s="66"/>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="D9" s="10">
         <v>0.02</v>
@@ -4003,7 +4015,7 @@
       <c r="A10" s="63"/>
       <c r="B10" s="66"/>
       <c r="C10" s="9" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D10" s="10">
         <v>0.02</v>
@@ -4020,7 +4032,7 @@
       <c r="A11" s="63"/>
       <c r="B11" s="66"/>
       <c r="C11" s="9" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D11" s="10">
         <v>0.02</v>
@@ -4037,7 +4049,7 @@
       <c r="A12" s="63"/>
       <c r="B12" s="66"/>
       <c r="C12" s="9" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D12" s="10">
         <v>0.02</v>
@@ -4054,7 +4066,7 @@
       <c r="A13" s="63"/>
       <c r="B13" s="66"/>
       <c r="C13" s="9" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="D13" s="10">
         <v>0.01</v>
@@ -4071,7 +4083,7 @@
       <c r="A14" s="63"/>
       <c r="B14" s="66"/>
       <c r="C14" s="9" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="D14" s="10">
         <v>0.01</v>
@@ -4088,7 +4100,7 @@
       <c r="A15" s="63"/>
       <c r="B15" s="66"/>
       <c r="C15" s="9" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="D15" s="10">
         <v>0.01</v>
@@ -4105,7 +4117,7 @@
       <c r="A16" s="63"/>
       <c r="B16" s="66"/>
       <c r="C16" s="9" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="D16" s="10">
         <v>0.01</v>
@@ -4122,7 +4134,7 @@
       <c r="A17" s="64"/>
       <c r="B17" s="66"/>
       <c r="C17" s="9" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="D17" s="10">
         <v>0.01</v>
@@ -4137,11 +4149,11 @@
     </row>
     <row r="18" spans="1:11" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="67" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="B18" s="68"/>
       <c r="C18" s="6" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="D18" s="5">
         <v>1</v>
@@ -4164,34 +4176,34 @@
     </row>
     <row r="20" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="I20" s="57" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A21" s="69"/>
       <c r="B21" s="24" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -4215,10 +4227,10 @@
       <c r="F22" s="2"/>
       <c r="I22" s="59"/>
       <c r="J22" s="19" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
@@ -4307,27 +4319,27 @@
       <c r="A1" s="60"/>
       <c r="B1" s="61"/>
       <c r="C1" s="11" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="D2" s="8">
         <v>0.5</v>
@@ -4344,7 +4356,7 @@
       <c r="A3" s="63"/>
       <c r="B3" s="65"/>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D3" s="8">
         <v>0.15</v>
@@ -4361,7 +4373,7 @@
       <c r="A4" s="63"/>
       <c r="B4" s="65"/>
       <c r="C4" s="7" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D4" s="8">
         <v>0.1</v>
@@ -4377,10 +4389,10 @@
     <row r="5" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
       <c r="B5" s="66" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D5" s="10">
         <v>0.04</v>
@@ -4397,7 +4409,7 @@
       <c r="A6" s="63"/>
       <c r="B6" s="66"/>
       <c r="C6" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="D6" s="10">
         <v>0.03</v>
@@ -4414,7 +4426,7 @@
       <c r="A7" s="63"/>
       <c r="B7" s="66"/>
       <c r="C7" s="9" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D7" s="10">
         <v>0.03</v>
@@ -4431,7 +4443,7 @@
       <c r="A8" s="63"/>
       <c r="B8" s="66"/>
       <c r="C8" s="9" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="D8" s="10">
         <v>0.02</v>
@@ -4448,7 +4460,7 @@
       <c r="A9" s="63"/>
       <c r="B9" s="66"/>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="D9" s="10">
         <v>0.02</v>
@@ -4465,7 +4477,7 @@
       <c r="A10" s="63"/>
       <c r="B10" s="66"/>
       <c r="C10" s="9" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D10" s="10">
         <v>0.02</v>
@@ -4482,7 +4494,7 @@
       <c r="A11" s="63"/>
       <c r="B11" s="66"/>
       <c r="C11" s="9" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D11" s="10">
         <v>0.02</v>
@@ -4499,7 +4511,7 @@
       <c r="A12" s="63"/>
       <c r="B12" s="66"/>
       <c r="C12" s="9" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D12" s="10">
         <v>0.02</v>
@@ -4516,7 +4528,7 @@
       <c r="A13" s="63"/>
       <c r="B13" s="66"/>
       <c r="C13" s="9" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="D13" s="10">
         <v>0.01</v>
@@ -4533,7 +4545,7 @@
       <c r="A14" s="63"/>
       <c r="B14" s="66"/>
       <c r="C14" s="9" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="D14" s="10">
         <v>0.01</v>
@@ -4550,7 +4562,7 @@
       <c r="A15" s="63"/>
       <c r="B15" s="66"/>
       <c r="C15" s="9" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="D15" s="10">
         <v>0.01</v>
@@ -4567,7 +4579,7 @@
       <c r="A16" s="63"/>
       <c r="B16" s="66"/>
       <c r="C16" s="9" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="D16" s="10">
         <v>0.01</v>
@@ -4584,7 +4596,7 @@
       <c r="A17" s="64"/>
       <c r="B17" s="66"/>
       <c r="C17" s="9" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="D17" s="10">
         <v>0.01</v>
@@ -4599,11 +4611,11 @@
     </row>
     <row r="18" spans="1:11" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="67" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="B18" s="68"/>
       <c r="C18" s="6" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="D18" s="5">
         <v>1</v>
@@ -4626,34 +4638,34 @@
     </row>
     <row r="20" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="I20" s="57" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A21" s="69"/>
       <c r="B21" s="24" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -4677,10 +4689,10 @@
       <c r="F22" s="2"/>
       <c r="I22" s="59"/>
       <c r="J22" s="19" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
@@ -4769,27 +4781,27 @@
       <c r="A1" s="60"/>
       <c r="B1" s="61"/>
       <c r="C1" s="11" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="D2" s="8">
         <v>0.5</v>
@@ -4806,7 +4818,7 @@
       <c r="A3" s="63"/>
       <c r="B3" s="65"/>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D3" s="8">
         <v>0.15</v>
@@ -4823,7 +4835,7 @@
       <c r="A4" s="63"/>
       <c r="B4" s="65"/>
       <c r="C4" s="7" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D4" s="8">
         <v>0.1</v>
@@ -4839,10 +4851,10 @@
     <row r="5" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
       <c r="B5" s="66" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D5" s="10">
         <v>0.04</v>
@@ -4859,7 +4871,7 @@
       <c r="A6" s="63"/>
       <c r="B6" s="66"/>
       <c r="C6" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="D6" s="10">
         <v>0.03</v>
@@ -4876,7 +4888,7 @@
       <c r="A7" s="63"/>
       <c r="B7" s="66"/>
       <c r="C7" s="9" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D7" s="10">
         <v>0.03</v>
@@ -4893,7 +4905,7 @@
       <c r="A8" s="63"/>
       <c r="B8" s="66"/>
       <c r="C8" s="9" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="D8" s="10">
         <v>0.02</v>
@@ -4910,7 +4922,7 @@
       <c r="A9" s="63"/>
       <c r="B9" s="66"/>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="D9" s="10">
         <v>0.02</v>
@@ -4927,7 +4939,7 @@
       <c r="A10" s="63"/>
       <c r="B10" s="66"/>
       <c r="C10" s="9" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D10" s="10">
         <v>0.02</v>
@@ -4944,7 +4956,7 @@
       <c r="A11" s="63"/>
       <c r="B11" s="66"/>
       <c r="C11" s="9" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D11" s="10">
         <v>0.02</v>
@@ -4961,7 +4973,7 @@
       <c r="A12" s="63"/>
       <c r="B12" s="66"/>
       <c r="C12" s="9" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D12" s="10">
         <v>0.02</v>
@@ -4978,7 +4990,7 @@
       <c r="A13" s="63"/>
       <c r="B13" s="66"/>
       <c r="C13" s="9" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="D13" s="10">
         <v>0.01</v>
@@ -4995,7 +5007,7 @@
       <c r="A14" s="63"/>
       <c r="B14" s="66"/>
       <c r="C14" s="9" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="D14" s="10">
         <v>0.01</v>
@@ -5012,7 +5024,7 @@
       <c r="A15" s="63"/>
       <c r="B15" s="66"/>
       <c r="C15" s="9" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="D15" s="10">
         <v>0.01</v>
@@ -5029,7 +5041,7 @@
       <c r="A16" s="63"/>
       <c r="B16" s="66"/>
       <c r="C16" s="9" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="D16" s="10">
         <v>0.01</v>
@@ -5046,7 +5058,7 @@
       <c r="A17" s="64"/>
       <c r="B17" s="66"/>
       <c r="C17" s="9" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="D17" s="10">
         <v>0.01</v>
@@ -5061,11 +5073,11 @@
     </row>
     <row r="18" spans="1:11" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="67" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="B18" s="68"/>
       <c r="C18" s="6" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="D18" s="5">
         <v>1</v>
@@ -5088,34 +5100,34 @@
     </row>
     <row r="20" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="I20" s="57" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A21" s="69"/>
       <c r="B21" s="24" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -5139,10 +5151,10 @@
       <c r="F22" s="2"/>
       <c r="I22" s="59"/>
       <c r="J22" s="19" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
@@ -5231,27 +5243,27 @@
       <c r="A1" s="60"/>
       <c r="B1" s="61"/>
       <c r="C1" s="11" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="D2" s="8">
         <v>0.5</v>
@@ -5268,7 +5280,7 @@
       <c r="A3" s="63"/>
       <c r="B3" s="65"/>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D3" s="8">
         <v>0.15</v>
@@ -5285,7 +5297,7 @@
       <c r="A4" s="63"/>
       <c r="B4" s="65"/>
       <c r="C4" s="7" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D4" s="8">
         <v>0.1</v>
@@ -5301,10 +5313,10 @@
     <row r="5" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
       <c r="B5" s="66" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D5" s="10">
         <v>0.04</v>
@@ -5321,7 +5333,7 @@
       <c r="A6" s="63"/>
       <c r="B6" s="66"/>
       <c r="C6" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="D6" s="10">
         <v>0.03</v>
@@ -5338,7 +5350,7 @@
       <c r="A7" s="63"/>
       <c r="B7" s="66"/>
       <c r="C7" s="9" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D7" s="10">
         <v>0.03</v>
@@ -5355,7 +5367,7 @@
       <c r="A8" s="63"/>
       <c r="B8" s="66"/>
       <c r="C8" s="9" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="D8" s="10">
         <v>0.02</v>
@@ -5372,7 +5384,7 @@
       <c r="A9" s="63"/>
       <c r="B9" s="66"/>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="D9" s="10">
         <v>0.02</v>
@@ -5389,7 +5401,7 @@
       <c r="A10" s="63"/>
       <c r="B10" s="66"/>
       <c r="C10" s="9" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D10" s="10">
         <v>0.02</v>
@@ -5406,7 +5418,7 @@
       <c r="A11" s="63"/>
       <c r="B11" s="66"/>
       <c r="C11" s="9" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D11" s="10">
         <v>0.02</v>
@@ -5423,7 +5435,7 @@
       <c r="A12" s="63"/>
       <c r="B12" s="66"/>
       <c r="C12" s="9" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D12" s="10">
         <v>0.02</v>
@@ -5440,7 +5452,7 @@
       <c r="A13" s="63"/>
       <c r="B13" s="66"/>
       <c r="C13" s="9" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="D13" s="10">
         <v>0.01</v>
@@ -5457,7 +5469,7 @@
       <c r="A14" s="63"/>
       <c r="B14" s="66"/>
       <c r="C14" s="9" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="D14" s="10">
         <v>0.01</v>
@@ -5474,7 +5486,7 @@
       <c r="A15" s="63"/>
       <c r="B15" s="66"/>
       <c r="C15" s="9" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="D15" s="10">
         <v>0.01</v>
@@ -5491,7 +5503,7 @@
       <c r="A16" s="63"/>
       <c r="B16" s="66"/>
       <c r="C16" s="9" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="D16" s="10">
         <v>0.01</v>
@@ -5508,7 +5520,7 @@
       <c r="A17" s="64"/>
       <c r="B17" s="66"/>
       <c r="C17" s="9" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="D17" s="10">
         <v>0.01</v>
@@ -5523,11 +5535,11 @@
     </row>
     <row r="18" spans="1:11" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="67" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="B18" s="68"/>
       <c r="C18" s="6" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="D18" s="5">
         <v>1</v>
@@ -5550,34 +5562,34 @@
     </row>
     <row r="20" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="I20" s="57" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A21" s="69"/>
       <c r="B21" s="24" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -5601,10 +5613,10 @@
       <c r="F22" s="2"/>
       <c r="I22" s="59"/>
       <c r="J22" s="19" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
@@ -5693,27 +5705,27 @@
       <c r="A1" s="60"/>
       <c r="B1" s="61"/>
       <c r="C1" s="11" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="D2" s="8">
         <v>0.5</v>
@@ -5730,7 +5742,7 @@
       <c r="A3" s="63"/>
       <c r="B3" s="65"/>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D3" s="8">
         <v>0.15</v>
@@ -5747,7 +5759,7 @@
       <c r="A4" s="63"/>
       <c r="B4" s="65"/>
       <c r="C4" s="7" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D4" s="8">
         <v>0.1</v>
@@ -5763,10 +5775,10 @@
     <row r="5" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
       <c r="B5" s="66" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D5" s="10">
         <v>0.04</v>
@@ -5783,7 +5795,7 @@
       <c r="A6" s="63"/>
       <c r="B6" s="66"/>
       <c r="C6" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="D6" s="10">
         <v>0.03</v>
@@ -5800,7 +5812,7 @@
       <c r="A7" s="63"/>
       <c r="B7" s="66"/>
       <c r="C7" s="9" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D7" s="10">
         <v>0.03</v>
@@ -5817,7 +5829,7 @@
       <c r="A8" s="63"/>
       <c r="B8" s="66"/>
       <c r="C8" s="9" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="D8" s="10">
         <v>0.02</v>
@@ -5834,7 +5846,7 @@
       <c r="A9" s="63"/>
       <c r="B9" s="66"/>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="D9" s="10">
         <v>0.02</v>
@@ -5851,7 +5863,7 @@
       <c r="A10" s="63"/>
       <c r="B10" s="66"/>
       <c r="C10" s="9" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D10" s="10">
         <v>0.02</v>
@@ -5868,7 +5880,7 @@
       <c r="A11" s="63"/>
       <c r="B11" s="66"/>
       <c r="C11" s="9" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D11" s="10">
         <v>0.02</v>
@@ -5885,7 +5897,7 @@
       <c r="A12" s="63"/>
       <c r="B12" s="66"/>
       <c r="C12" s="9" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D12" s="10">
         <v>0.02</v>
@@ -5902,7 +5914,7 @@
       <c r="A13" s="63"/>
       <c r="B13" s="66"/>
       <c r="C13" s="9" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="D13" s="10">
         <v>0.01</v>
@@ -5919,7 +5931,7 @@
       <c r="A14" s="63"/>
       <c r="B14" s="66"/>
       <c r="C14" s="9" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="D14" s="10">
         <v>0.01</v>
@@ -5936,7 +5948,7 @@
       <c r="A15" s="63"/>
       <c r="B15" s="66"/>
       <c r="C15" s="9" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="D15" s="10">
         <v>0.01</v>
@@ -5953,7 +5965,7 @@
       <c r="A16" s="63"/>
       <c r="B16" s="66"/>
       <c r="C16" s="9" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="D16" s="10">
         <v>0.01</v>
@@ -5970,7 +5982,7 @@
       <c r="A17" s="64"/>
       <c r="B17" s="66"/>
       <c r="C17" s="9" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="D17" s="10">
         <v>0.01</v>
@@ -5985,11 +5997,11 @@
     </row>
     <row r="18" spans="1:11" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="67" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="B18" s="68"/>
       <c r="C18" s="6" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="D18" s="5">
         <v>1</v>
@@ -6012,34 +6024,34 @@
     </row>
     <row r="20" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="I20" s="57" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A21" s="69"/>
       <c r="B21" s="24" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -6063,10 +6075,10 @@
       <c r="F22" s="2"/>
       <c r="I22" s="59"/>
       <c r="J22" s="19" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
@@ -6155,27 +6167,27 @@
       <c r="A1" s="60"/>
       <c r="B1" s="61"/>
       <c r="C1" s="11" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="D2" s="8">
         <v>0.5</v>
@@ -6192,7 +6204,7 @@
       <c r="A3" s="63"/>
       <c r="B3" s="65"/>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D3" s="8">
         <v>0.15</v>
@@ -6209,7 +6221,7 @@
       <c r="A4" s="63"/>
       <c r="B4" s="65"/>
       <c r="C4" s="7" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D4" s="8">
         <v>0.1</v>
@@ -6225,10 +6237,10 @@
     <row r="5" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
       <c r="B5" s="66" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D5" s="10">
         <v>0.04</v>
@@ -6245,7 +6257,7 @@
       <c r="A6" s="63"/>
       <c r="B6" s="66"/>
       <c r="C6" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="D6" s="10">
         <v>0.03</v>
@@ -6262,7 +6274,7 @@
       <c r="A7" s="63"/>
       <c r="B7" s="66"/>
       <c r="C7" s="9" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D7" s="10">
         <v>0.03</v>
@@ -6279,7 +6291,7 @@
       <c r="A8" s="63"/>
       <c r="B8" s="66"/>
       <c r="C8" s="9" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="D8" s="10">
         <v>0.02</v>
@@ -6296,7 +6308,7 @@
       <c r="A9" s="63"/>
       <c r="B9" s="66"/>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="D9" s="10">
         <v>0.02</v>
@@ -6313,7 +6325,7 @@
       <c r="A10" s="63"/>
       <c r="B10" s="66"/>
       <c r="C10" s="9" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D10" s="10">
         <v>0.02</v>
@@ -6330,7 +6342,7 @@
       <c r="A11" s="63"/>
       <c r="B11" s="66"/>
       <c r="C11" s="9" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D11" s="10">
         <v>0.02</v>
@@ -6347,7 +6359,7 @@
       <c r="A12" s="63"/>
       <c r="B12" s="66"/>
       <c r="C12" s="9" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D12" s="10">
         <v>0.02</v>
@@ -6364,7 +6376,7 @@
       <c r="A13" s="63"/>
       <c r="B13" s="66"/>
       <c r="C13" s="9" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="D13" s="10">
         <v>0.01</v>
@@ -6381,7 +6393,7 @@
       <c r="A14" s="63"/>
       <c r="B14" s="66"/>
       <c r="C14" s="9" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="D14" s="10">
         <v>0.01</v>
@@ -6398,7 +6410,7 @@
       <c r="A15" s="63"/>
       <c r="B15" s="66"/>
       <c r="C15" s="9" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="D15" s="10">
         <v>0.01</v>
@@ -6415,7 +6427,7 @@
       <c r="A16" s="63"/>
       <c r="B16" s="66"/>
       <c r="C16" s="9" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="D16" s="10">
         <v>0.01</v>
@@ -6432,7 +6444,7 @@
       <c r="A17" s="64"/>
       <c r="B17" s="66"/>
       <c r="C17" s="9" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="D17" s="10">
         <v>0.01</v>
@@ -6447,11 +6459,11 @@
     </row>
     <row r="18" spans="1:11" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="67" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="B18" s="68"/>
       <c r="C18" s="6" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="D18" s="5">
         <v>1</v>
@@ -6474,34 +6486,34 @@
     </row>
     <row r="20" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="I20" s="57" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A21" s="69"/>
       <c r="B21" s="24" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -6525,10 +6537,10 @@
       <c r="F22" s="2"/>
       <c r="I22" s="59"/>
       <c r="J22" s="19" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
@@ -6635,27 +6647,27 @@
       <c r="A1" s="60"/>
       <c r="B1" s="61"/>
       <c r="C1" s="11" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="D2" s="8">
         <v>0.5</v>
@@ -6672,7 +6684,7 @@
       <c r="A3" s="63"/>
       <c r="B3" s="65"/>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D3" s="8">
         <v>0.15</v>
@@ -6689,7 +6701,7 @@
       <c r="A4" s="63"/>
       <c r="B4" s="65"/>
       <c r="C4" s="7" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D4" s="8">
         <v>0.1</v>
@@ -6705,10 +6717,10 @@
     <row r="5" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
       <c r="B5" s="66" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D5" s="10">
         <v>0.04</v>
@@ -6725,7 +6737,7 @@
       <c r="A6" s="63"/>
       <c r="B6" s="66"/>
       <c r="C6" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="D6" s="10">
         <v>0.03</v>
@@ -6742,7 +6754,7 @@
       <c r="A7" s="63"/>
       <c r="B7" s="66"/>
       <c r="C7" s="9" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D7" s="10">
         <v>0.03</v>
@@ -6759,7 +6771,7 @@
       <c r="A8" s="63"/>
       <c r="B8" s="66"/>
       <c r="C8" s="9" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="D8" s="10">
         <v>0.02</v>
@@ -6776,7 +6788,7 @@
       <c r="A9" s="63"/>
       <c r="B9" s="66"/>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="D9" s="10">
         <v>0.02</v>
@@ -6793,7 +6805,7 @@
       <c r="A10" s="63"/>
       <c r="B10" s="66"/>
       <c r="C10" s="9" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D10" s="10">
         <v>0.02</v>
@@ -6810,7 +6822,7 @@
       <c r="A11" s="63"/>
       <c r="B11" s="66"/>
       <c r="C11" s="9" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D11" s="10">
         <v>0.02</v>
@@ -6827,7 +6839,7 @@
       <c r="A12" s="63"/>
       <c r="B12" s="66"/>
       <c r="C12" s="9" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D12" s="10">
         <v>0.02</v>
@@ -6844,7 +6856,7 @@
       <c r="A13" s="63"/>
       <c r="B13" s="66"/>
       <c r="C13" s="9" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="D13" s="10">
         <v>0.01</v>
@@ -6861,7 +6873,7 @@
       <c r="A14" s="63"/>
       <c r="B14" s="66"/>
       <c r="C14" s="9" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="D14" s="10">
         <v>0.01</v>
@@ -6878,7 +6890,7 @@
       <c r="A15" s="63"/>
       <c r="B15" s="66"/>
       <c r="C15" s="9" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="D15" s="10">
         <v>0.01</v>
@@ -6895,7 +6907,7 @@
       <c r="A16" s="63"/>
       <c r="B16" s="66"/>
       <c r="C16" s="9" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="D16" s="10">
         <v>0.01</v>
@@ -6912,7 +6924,7 @@
       <c r="A17" s="64"/>
       <c r="B17" s="66"/>
       <c r="C17" s="9" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="D17" s="10">
         <v>0.01</v>
@@ -6927,11 +6939,11 @@
     </row>
     <row r="18" spans="1:11" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="67" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="B18" s="68"/>
       <c r="C18" s="6" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="D18" s="5">
         <v>1</v>
@@ -6954,34 +6966,34 @@
     </row>
     <row r="20" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="I20" s="57" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A21" s="69"/>
       <c r="B21" s="24" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -7005,10 +7017,10 @@
       <c r="F22" s="2"/>
       <c r="I22" s="59"/>
       <c r="J22" s="19" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
@@ -7122,27 +7134,27 @@
       <c r="A1" s="60"/>
       <c r="B1" s="61"/>
       <c r="C1" s="11" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="D2" s="8">
         <v>0.5</v>
@@ -7159,7 +7171,7 @@
       <c r="A3" s="63"/>
       <c r="B3" s="65"/>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D3" s="8">
         <v>0.15</v>
@@ -7176,7 +7188,7 @@
       <c r="A4" s="63"/>
       <c r="B4" s="65"/>
       <c r="C4" s="7" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D4" s="8">
         <v>0.1</v>
@@ -7192,10 +7204,10 @@
     <row r="5" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
       <c r="B5" s="66" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D5" s="10">
         <v>0.04</v>
@@ -7212,7 +7224,7 @@
       <c r="A6" s="63"/>
       <c r="B6" s="66"/>
       <c r="C6" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="D6" s="10">
         <v>0.03</v>
@@ -7229,7 +7241,7 @@
       <c r="A7" s="63"/>
       <c r="B7" s="66"/>
       <c r="C7" s="9" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D7" s="10">
         <v>0.03</v>
@@ -7246,7 +7258,7 @@
       <c r="A8" s="63"/>
       <c r="B8" s="66"/>
       <c r="C8" s="9" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="D8" s="10">
         <v>0.02</v>
@@ -7263,7 +7275,7 @@
       <c r="A9" s="63"/>
       <c r="B9" s="66"/>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="D9" s="10">
         <v>0.02</v>
@@ -7280,7 +7292,7 @@
       <c r="A10" s="63"/>
       <c r="B10" s="66"/>
       <c r="C10" s="9" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D10" s="10">
         <v>0.02</v>
@@ -7297,7 +7309,7 @@
       <c r="A11" s="63"/>
       <c r="B11" s="66"/>
       <c r="C11" s="9" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D11" s="10">
         <v>0.02</v>
@@ -7314,7 +7326,7 @@
       <c r="A12" s="63"/>
       <c r="B12" s="66"/>
       <c r="C12" s="9" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D12" s="10">
         <v>0.02</v>
@@ -7331,7 +7343,7 @@
       <c r="A13" s="63"/>
       <c r="B13" s="66"/>
       <c r="C13" s="9" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="D13" s="10">
         <v>0.01</v>
@@ -7348,7 +7360,7 @@
       <c r="A14" s="63"/>
       <c r="B14" s="66"/>
       <c r="C14" s="9" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="D14" s="10">
         <v>0.01</v>
@@ -7365,7 +7377,7 @@
       <c r="A15" s="63"/>
       <c r="B15" s="66"/>
       <c r="C15" s="9" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="D15" s="10">
         <v>0.01</v>
@@ -7382,7 +7394,7 @@
       <c r="A16" s="63"/>
       <c r="B16" s="66"/>
       <c r="C16" s="9" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="D16" s="10">
         <v>0.01</v>
@@ -7399,7 +7411,7 @@
       <c r="A17" s="64"/>
       <c r="B17" s="66"/>
       <c r="C17" s="9" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="D17" s="10">
         <v>0.01</v>
@@ -7414,11 +7426,11 @@
     </row>
     <row r="18" spans="1:11" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="67" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="B18" s="68"/>
       <c r="C18" s="6" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="D18" s="5">
         <v>1</v>
@@ -7441,34 +7453,34 @@
     </row>
     <row r="20" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="I20" s="57" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A21" s="69"/>
       <c r="B21" s="24" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -7492,10 +7504,10 @@
       <c r="F22" s="2"/>
       <c r="I22" s="59"/>
       <c r="J22" s="19" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
@@ -7584,27 +7596,27 @@
       <c r="A1" s="60"/>
       <c r="B1" s="61"/>
       <c r="C1" s="11" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="D2" s="8">
         <v>0.5</v>
@@ -7621,7 +7633,7 @@
       <c r="A3" s="63"/>
       <c r="B3" s="65"/>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D3" s="8">
         <v>0.15</v>
@@ -7638,7 +7650,7 @@
       <c r="A4" s="63"/>
       <c r="B4" s="65"/>
       <c r="C4" s="7" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D4" s="8">
         <v>0.1</v>
@@ -7654,10 +7666,10 @@
     <row r="5" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
       <c r="B5" s="66" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D5" s="10">
         <v>0.04</v>
@@ -7674,7 +7686,7 @@
       <c r="A6" s="63"/>
       <c r="B6" s="66"/>
       <c r="C6" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="D6" s="10">
         <v>0.03</v>
@@ -7691,7 +7703,7 @@
       <c r="A7" s="63"/>
       <c r="B7" s="66"/>
       <c r="C7" s="9" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D7" s="10">
         <v>0.03</v>
@@ -7708,7 +7720,7 @@
       <c r="A8" s="63"/>
       <c r="B8" s="66"/>
       <c r="C8" s="9" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="D8" s="10">
         <v>0.02</v>
@@ -7725,7 +7737,7 @@
       <c r="A9" s="63"/>
       <c r="B9" s="66"/>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="D9" s="10">
         <v>0.02</v>
@@ -7742,7 +7754,7 @@
       <c r="A10" s="63"/>
       <c r="B10" s="66"/>
       <c r="C10" s="9" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D10" s="10">
         <v>0.02</v>
@@ -7759,7 +7771,7 @@
       <c r="A11" s="63"/>
       <c r="B11" s="66"/>
       <c r="C11" s="9" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D11" s="10">
         <v>0.02</v>
@@ -7776,7 +7788,7 @@
       <c r="A12" s="63"/>
       <c r="B12" s="66"/>
       <c r="C12" s="9" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D12" s="10">
         <v>0.02</v>
@@ -7793,7 +7805,7 @@
       <c r="A13" s="63"/>
       <c r="B13" s="66"/>
       <c r="C13" s="9" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="D13" s="10">
         <v>0.01</v>
@@ -7810,7 +7822,7 @@
       <c r="A14" s="63"/>
       <c r="B14" s="66"/>
       <c r="C14" s="9" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="D14" s="10">
         <v>0.01</v>
@@ -7827,7 +7839,7 @@
       <c r="A15" s="63"/>
       <c r="B15" s="66"/>
       <c r="C15" s="9" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="D15" s="10">
         <v>0.01</v>
@@ -7844,7 +7856,7 @@
       <c r="A16" s="63"/>
       <c r="B16" s="66"/>
       <c r="C16" s="9" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="D16" s="10">
         <v>0.01</v>
@@ -7861,7 +7873,7 @@
       <c r="A17" s="64"/>
       <c r="B17" s="66"/>
       <c r="C17" s="9" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="D17" s="10">
         <v>0.01</v>
@@ -7876,11 +7888,11 @@
     </row>
     <row r="18" spans="1:11" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="67" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="B18" s="68"/>
       <c r="C18" s="6" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="D18" s="5">
         <v>1</v>
@@ -7903,34 +7915,34 @@
     </row>
     <row r="20" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="I20" s="57" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A21" s="69"/>
       <c r="B21" s="24" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -7954,10 +7966,10 @@
       <c r="F22" s="2"/>
       <c r="I22" s="59"/>
       <c r="J22" s="19" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
@@ -8046,27 +8058,27 @@
       <c r="A1" s="60"/>
       <c r="B1" s="61"/>
       <c r="C1" s="11" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="D2" s="8">
         <v>0.5</v>
@@ -8083,7 +8095,7 @@
       <c r="A3" s="63"/>
       <c r="B3" s="65"/>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D3" s="8">
         <v>0.15</v>
@@ -8100,7 +8112,7 @@
       <c r="A4" s="63"/>
       <c r="B4" s="65"/>
       <c r="C4" s="7" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D4" s="8">
         <v>0.1</v>
@@ -8116,10 +8128,10 @@
     <row r="5" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
       <c r="B5" s="66" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D5" s="10">
         <v>0.04</v>
@@ -8136,7 +8148,7 @@
       <c r="A6" s="63"/>
       <c r="B6" s="66"/>
       <c r="C6" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="D6" s="10">
         <v>0.03</v>
@@ -8153,7 +8165,7 @@
       <c r="A7" s="63"/>
       <c r="B7" s="66"/>
       <c r="C7" s="9" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D7" s="10">
         <v>0.03</v>
@@ -8170,7 +8182,7 @@
       <c r="A8" s="63"/>
       <c r="B8" s="66"/>
       <c r="C8" s="9" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="D8" s="10">
         <v>0.02</v>
@@ -8187,7 +8199,7 @@
       <c r="A9" s="63"/>
       <c r="B9" s="66"/>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="D9" s="10">
         <v>0.02</v>
@@ -8204,7 +8216,7 @@
       <c r="A10" s="63"/>
       <c r="B10" s="66"/>
       <c r="C10" s="9" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D10" s="10">
         <v>0.02</v>
@@ -8221,7 +8233,7 @@
       <c r="A11" s="63"/>
       <c r="B11" s="66"/>
       <c r="C11" s="9" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D11" s="10">
         <v>0.02</v>
@@ -8238,7 +8250,7 @@
       <c r="A12" s="63"/>
       <c r="B12" s="66"/>
       <c r="C12" s="9" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D12" s="10">
         <v>0.02</v>
@@ -8255,7 +8267,7 @@
       <c r="A13" s="63"/>
       <c r="B13" s="66"/>
       <c r="C13" s="9" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="D13" s="10">
         <v>0.01</v>
@@ -8272,7 +8284,7 @@
       <c r="A14" s="63"/>
       <c r="B14" s="66"/>
       <c r="C14" s="9" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="D14" s="10">
         <v>0.01</v>
@@ -8289,7 +8301,7 @@
       <c r="A15" s="63"/>
       <c r="B15" s="66"/>
       <c r="C15" s="9" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="D15" s="10">
         <v>0.01</v>
@@ -8306,7 +8318,7 @@
       <c r="A16" s="63"/>
       <c r="B16" s="66"/>
       <c r="C16" s="9" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="D16" s="10">
         <v>0.01</v>
@@ -8323,7 +8335,7 @@
       <c r="A17" s="64"/>
       <c r="B17" s="66"/>
       <c r="C17" s="9" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="D17" s="10">
         <v>0.01</v>
@@ -8338,11 +8350,11 @@
     </row>
     <row r="18" spans="1:11" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="67" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="B18" s="68"/>
       <c r="C18" s="6" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="D18" s="5">
         <v>1</v>
@@ -8365,34 +8377,34 @@
     </row>
     <row r="20" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="I20" s="57" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A21" s="69"/>
       <c r="B21" s="24" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -8416,10 +8428,10 @@
       <c r="F22" s="2"/>
       <c r="I22" s="59"/>
       <c r="J22" s="19" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
@@ -8508,27 +8520,27 @@
       <c r="A1" s="60"/>
       <c r="B1" s="61"/>
       <c r="C1" s="11" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="D2" s="8">
         <v>0.5</v>
@@ -8545,7 +8557,7 @@
       <c r="A3" s="63"/>
       <c r="B3" s="65"/>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D3" s="8">
         <v>0.15</v>
@@ -8562,7 +8574,7 @@
       <c r="A4" s="63"/>
       <c r="B4" s="65"/>
       <c r="C4" s="7" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D4" s="8">
         <v>0.1</v>
@@ -8578,10 +8590,10 @@
     <row r="5" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
       <c r="B5" s="66" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D5" s="10">
         <v>0.04</v>
@@ -8598,7 +8610,7 @@
       <c r="A6" s="63"/>
       <c r="B6" s="66"/>
       <c r="C6" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="D6" s="10">
         <v>0.03</v>
@@ -8615,7 +8627,7 @@
       <c r="A7" s="63"/>
       <c r="B7" s="66"/>
       <c r="C7" s="9" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D7" s="10">
         <v>0.03</v>
@@ -8632,7 +8644,7 @@
       <c r="A8" s="63"/>
       <c r="B8" s="66"/>
       <c r="C8" s="9" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="D8" s="10">
         <v>0.02</v>
@@ -8649,7 +8661,7 @@
       <c r="A9" s="63"/>
       <c r="B9" s="66"/>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="D9" s="10">
         <v>0.02</v>
@@ -8666,7 +8678,7 @@
       <c r="A10" s="63"/>
       <c r="B10" s="66"/>
       <c r="C10" s="9" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D10" s="10">
         <v>0.02</v>
@@ -8683,7 +8695,7 @@
       <c r="A11" s="63"/>
       <c r="B11" s="66"/>
       <c r="C11" s="9" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D11" s="10">
         <v>0.02</v>
@@ -8700,7 +8712,7 @@
       <c r="A12" s="63"/>
       <c r="B12" s="66"/>
       <c r="C12" s="9" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D12" s="10">
         <v>0.02</v>
@@ -8717,7 +8729,7 @@
       <c r="A13" s="63"/>
       <c r="B13" s="66"/>
       <c r="C13" s="9" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="D13" s="10">
         <v>0.01</v>
@@ -8734,7 +8746,7 @@
       <c r="A14" s="63"/>
       <c r="B14" s="66"/>
       <c r="C14" s="9" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="D14" s="10">
         <v>0.01</v>
@@ -8751,7 +8763,7 @@
       <c r="A15" s="63"/>
       <c r="B15" s="66"/>
       <c r="C15" s="9" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="D15" s="10">
         <v>0.01</v>
@@ -8768,7 +8780,7 @@
       <c r="A16" s="63"/>
       <c r="B16" s="66"/>
       <c r="C16" s="9" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="D16" s="10">
         <v>0.01</v>
@@ -8785,7 +8797,7 @@
       <c r="A17" s="64"/>
       <c r="B17" s="66"/>
       <c r="C17" s="9" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="D17" s="10">
         <v>0.01</v>
@@ -8800,11 +8812,11 @@
     </row>
     <row r="18" spans="1:11" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="67" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="B18" s="68"/>
       <c r="C18" s="6" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="D18" s="5">
         <v>1</v>
@@ -8827,34 +8839,34 @@
     </row>
     <row r="20" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="I20" s="57" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A21" s="69"/>
       <c r="B21" s="24" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -8878,10 +8890,10 @@
       <c r="F22" s="2"/>
       <c r="I22" s="59"/>
       <c r="J22" s="19" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
@@ -8970,27 +8982,27 @@
       <c r="A1" s="60"/>
       <c r="B1" s="61"/>
       <c r="C1" s="11" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="D2" s="8">
         <v>0.5</v>
@@ -9007,7 +9019,7 @@
       <c r="A3" s="63"/>
       <c r="B3" s="65"/>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D3" s="8">
         <v>0.15</v>
@@ -9024,7 +9036,7 @@
       <c r="A4" s="63"/>
       <c r="B4" s="65"/>
       <c r="C4" s="7" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D4" s="8">
         <v>0.1</v>
@@ -9040,10 +9052,10 @@
     <row r="5" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
       <c r="B5" s="66" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D5" s="10">
         <v>0.04</v>
@@ -9060,7 +9072,7 @@
       <c r="A6" s="63"/>
       <c r="B6" s="66"/>
       <c r="C6" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="D6" s="10">
         <v>0.03</v>
@@ -9077,7 +9089,7 @@
       <c r="A7" s="63"/>
       <c r="B7" s="66"/>
       <c r="C7" s="9" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D7" s="10">
         <v>0.03</v>
@@ -9094,7 +9106,7 @@
       <c r="A8" s="63"/>
       <c r="B8" s="66"/>
       <c r="C8" s="9" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="D8" s="10">
         <v>0.02</v>
@@ -9111,7 +9123,7 @@
       <c r="A9" s="63"/>
       <c r="B9" s="66"/>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="D9" s="10">
         <v>0.02</v>
@@ -9128,7 +9140,7 @@
       <c r="A10" s="63"/>
       <c r="B10" s="66"/>
       <c r="C10" s="9" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D10" s="10">
         <v>0.02</v>
@@ -9145,7 +9157,7 @@
       <c r="A11" s="63"/>
       <c r="B11" s="66"/>
       <c r="C11" s="9" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D11" s="10">
         <v>0.02</v>
@@ -9162,7 +9174,7 @@
       <c r="A12" s="63"/>
       <c r="B12" s="66"/>
       <c r="C12" s="9" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D12" s="10">
         <v>0.02</v>
@@ -9179,7 +9191,7 @@
       <c r="A13" s="63"/>
       <c r="B13" s="66"/>
       <c r="C13" s="9" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="D13" s="10">
         <v>0.01</v>
@@ -9196,7 +9208,7 @@
       <c r="A14" s="63"/>
       <c r="B14" s="66"/>
       <c r="C14" s="9" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="D14" s="10">
         <v>0.01</v>
@@ -9213,7 +9225,7 @@
       <c r="A15" s="63"/>
       <c r="B15" s="66"/>
       <c r="C15" s="9" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="D15" s="10">
         <v>0.01</v>
@@ -9230,7 +9242,7 @@
       <c r="A16" s="63"/>
       <c r="B16" s="66"/>
       <c r="C16" s="9" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="D16" s="10">
         <v>0.01</v>
@@ -9247,7 +9259,7 @@
       <c r="A17" s="64"/>
       <c r="B17" s="66"/>
       <c r="C17" s="9" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="D17" s="10">
         <v>0.01</v>
@@ -9262,11 +9274,11 @@
     </row>
     <row r="18" spans="1:11" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="67" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="B18" s="68"/>
       <c r="C18" s="6" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="D18" s="5">
         <v>1</v>
@@ -9289,34 +9301,34 @@
     </row>
     <row r="20" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="I20" s="57" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A21" s="69"/>
       <c r="B21" s="24" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>74</v>
+        <v>111</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -9340,10 +9352,10 @@
       <c r="F22" s="2"/>
       <c r="I22" s="59"/>
       <c r="J22" s="19" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
@@ -9432,27 +9444,27 @@
       <c r="A1" s="60"/>
       <c r="B1" s="61"/>
       <c r="C1" s="11" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="D2" s="8">
         <v>0.5</v>
@@ -9469,7 +9481,7 @@
       <c r="A3" s="63"/>
       <c r="B3" s="65"/>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D3" s="8">
         <v>0.15</v>
@@ -9486,7 +9498,7 @@
       <c r="A4" s="63"/>
       <c r="B4" s="65"/>
       <c r="C4" s="7" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D4" s="8">
         <v>0.1</v>
@@ -9502,10 +9514,10 @@
     <row r="5" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
       <c r="B5" s="66" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="D5" s="10">
         <v>0.04</v>
@@ -9522,7 +9534,7 @@
       <c r="A6" s="63"/>
       <c r="B6" s="66"/>
       <c r="C6" s="9" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="D6" s="10">
         <v>0.03</v>
@@ -9539,7 +9551,7 @@
       <c r="A7" s="63"/>
       <c r="B7" s="66"/>
       <c r="C7" s="9" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D7" s="10">
         <v>0.03</v>
@@ -9556,7 +9568,7 @@
       <c r="A8" s="63"/>
       <c r="B8" s="66"/>
       <c r="C8" s="9" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="D8" s="10">
         <v>0.02</v>
@@ -9573,7 +9585,7 @@
       <c r="A9" s="63"/>
       <c r="B9" s="66"/>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="D9" s="10">
         <v>0.02</v>
@@ -9590,7 +9602,7 @@
       <c r="A10" s="63"/>
       <c r="B10" s="66"/>
       <c r="C10" s="9" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D10" s="10">
         <v>0.02</v>
@@ -9607,7 +9619,7 @@
       <c r="A11" s="63"/>
       <c r="B11" s="66"/>
       <c r="C11" s="9" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D11" s="10">
         <v>0.02</v>
@@ -9624,7 +9636,7 @@
       <c r="A12" s="63"/>
       <c r="B12" s="66"/>
       <c r="C12" s="9" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D12" s="10">
         <v>0.02</v>
@@ -9641,7 +9653,7 @@
       <c r="A13" s="63"/>
       <c r="B13" s="66"/>
       <c r="C13" s="9" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="D13" s="10">
         <v>0.01</v>
@@ -9658,7 +9670,7 @@
       <c r="A14" s="63"/>
       <c r="B14" s="66"/>
       <c r="C14" s="9" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="D14" s="10">
         <v>0.01</v>
@@ -9675,7 +9687,7 @@
       <c r="A15" s="63"/>
       <c r="B15" s="66"/>
       <c r="C15" s="9" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="D15" s="10">
         <v>0.01</v>
@@ -9692,7 +9704,7 @@
       <c r="A16" s="63"/>
       <c r="B16" s="66"/>
       <c r="C16" s="9" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="D16" s="10">
         <v>0.01</v>
@@ -9709,7 +9721,7 @@
       <c r="A17" s="64"/>
       <c r="B17" s="66"/>
       <c r="C17" s="9" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="D17" s="10">
         <v>0.01</v>
@@ -9724,11 +9736,11 @@
     </row>
     <row r="18" spans="1:11" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="67" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="B18" s="68"/>
       <c r="C18" s="6" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="D18" s="5">
         <v>1</v>
@@ -9751,34 +9763,34 @@
     </row>
     <row r="20" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="I20" s="57" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A21" s="69"/>
       <c r="B21" s="24" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -9802,10 +9814,10 @@
       <c r="F22" s="2"/>
       <c r="I22" s="59"/>
       <c r="J22" s="19" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">

</xml_diff>